<commit_message>
Added new suite assertions
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-suitemap.xlsx
+++ b/test-data/webanalytics-suitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B677EC8A-94BF-4147-8AB8-48480D66C8A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5E1B393-5FA2-490C-AFE7-D0D465299A48}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>ncidevelopment</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>DevSuite</t>
+  </si>
+  <si>
+    <t>Suite</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941920-D2D7-425D-AAC9-2581B925B1AF}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
@@ -501,143 +504,194 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
       <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>